<commit_message>
Android paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4034CA39-F95E-4FA8-9135-9B7C44363E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF648006-5C0F-4917-8984-ACFFB713747B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Android Application" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -49,6 +50,24 @@
   </si>
   <si>
     <t>Project Development using Java 2021</t>
+  </si>
+  <si>
+    <t>Flutter &amp; Dart - The Complete Guide [2021 Edition]</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/learn-flutter-dart-to-build-ios-android-apps/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/social-networking-android-app-development-from-scratch/</t>
+  </si>
+  <si>
+    <t>How to make a Social Networking app -Android App Development</t>
+  </si>
+  <si>
+    <t>Android App Development Masterclass using Kotlin</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/android-oreo-kotlin-app-masterclass/</t>
   </si>
 </sst>
 </file>
@@ -402,17 +421,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B039CD-88E5-4E86-BFC7-B084BD245489}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="79" customWidth="1"/>
-    <col min="3" max="3" width="97.77734375" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -420,7 +439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -428,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -436,12 +455,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6810214A-8824-42FE-A3A6-41C4FD4021BF}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="72.85546875" customWidth="1"/>
+    <col min="3" max="3" width="128.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project based paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884A6B2A-9E10-4D96-B121-0A79DEA0204F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96C2C49-6C01-426B-9964-B8A69717E20C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Android Application" sheetId="2" r:id="rId2"/>
     <sheet name="Python" sheetId="3" r:id="rId3"/>
+    <sheet name="Projects" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -129,6 +130,30 @@
   </si>
   <si>
     <t>The Complete 2021 Flutter Development Bootcamp with Dart</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/100-days-of-code/</t>
+  </si>
+  <si>
+    <t>100 Days of Code - The Complete Python Pro Bootcamp for 2021</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/50-projects-50-days/</t>
+  </si>
+  <si>
+    <t>50 Projects In 50 Days - HTML, CSS &amp; JavaScript</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/web-projects-with-vanilla-javascript/</t>
+  </si>
+  <si>
+    <t>20 Web Projects With Vanilla JavaScript</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/electron-from-scratch/</t>
+  </si>
+  <si>
+    <t>Electron From Scratch: Build Desktop Apps With JavaScript</t>
   </si>
 </sst>
 </file>
@@ -533,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6810214A-8824-42FE-A3A6-41C4FD4021BF}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -582,10 +607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2773076E-175D-422E-B3B7-B91BC5516429}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,6 +691,57 @@
         <v>30</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D41AAE-5841-4A02-8EA4-8A7C0835E48E}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="91.5703125" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
JavaScript Framework based paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96C2C49-6C01-426B-9964-B8A69717E20C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E2C849-88BE-4FF0-8FE1-018346F7F257}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Android Application" sheetId="2" r:id="rId2"/>
     <sheet name="Python" sheetId="3" r:id="rId3"/>
     <sheet name="Projects" sheetId="4" r:id="rId4"/>
+    <sheet name="Framework" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -154,6 +155,18 @@
   </si>
   <si>
     <t>Electron From Scratch: Build Desktop Apps With JavaScript</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/angular-material-masterclass/</t>
+  </si>
+  <si>
+    <t>Angular Material: Ultimate Masterclass With Angular 9 (2020)</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/complete-react-course-w-hooks-react-router-redux-usecontext/</t>
+  </si>
+  <si>
+    <t>React - The Complete Guide with React Hook Redux 2021 in 4hr</t>
   </si>
 </sst>
 </file>
@@ -708,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D41AAE-5841-4A02-8EA4-8A7C0835E48E}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -745,4 +758,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD870DED-0179-42AB-8FFF-BE124EB6C140}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="100.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
JavaScript paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E2C849-88BE-4FF0-8FE1-018346F7F257}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FD29DF-18F1-4345-9B85-4B7994D53E9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Python" sheetId="3" r:id="rId3"/>
     <sheet name="Projects" sheetId="4" r:id="rId4"/>
     <sheet name="Framework" sheetId="5" r:id="rId5"/>
+    <sheet name="JavaScript" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -167,6 +168,12 @@
   </si>
   <si>
     <t>React - The Complete Guide with React Hook Redux 2021 in 4hr</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/ultimate-javascript-leetcode-interview-bootcamp/</t>
+  </si>
+  <si>
+    <t>JavaScript &amp; LeetCode | The Interview Bootcamp</t>
   </si>
 </sst>
 </file>
@@ -764,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD870DED-0179-42AB-8FFF-BE124EB6C140}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -793,4 +800,31 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C409B36-44BD-4ED2-A6DC-F7FC64FCD548}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="100.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
API development and testing paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FD29DF-18F1-4345-9B85-4B7994D53E9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2741B0DD-A255-4372-A8D3-35AA296B6879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Projects" sheetId="4" r:id="rId4"/>
     <sheet name="Framework" sheetId="5" r:id="rId5"/>
     <sheet name="JavaScript" sheetId="6" r:id="rId6"/>
+    <sheet name="API Dev and Testing" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -174,6 +175,18 @@
   </si>
   <si>
     <t>JavaScript &amp; LeetCode | The Interview Bootcamp</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/postman-the-complete-guide/</t>
+  </si>
+  <si>
+    <t>Postman: The Complete Guide - REST API Testing</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/django-rest-framework/</t>
+  </si>
+  <si>
+    <t>Build REST APIs with Django REST Framework and Python</t>
   </si>
 </sst>
 </file>
@@ -806,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C409B36-44BD-4ED2-A6DC-F7FC64FCD548}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -827,4 +840,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB6258B-92E2-456A-930B-3F7624ECCE6F}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Certification paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2741B0DD-A255-4372-A8D3-35AA296B6879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6525A8D8-F890-4D93-957E-ABC0C97559C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Framework" sheetId="5" r:id="rId5"/>
     <sheet name="JavaScript" sheetId="6" r:id="rId6"/>
     <sheet name="API Dev and Testing" sheetId="7" r:id="rId7"/>
+    <sheet name="Certification" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -187,6 +188,30 @@
   </si>
   <si>
     <t>Build REST APIs with Django REST Framework and Python</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/pentestplus/</t>
+  </si>
+  <si>
+    <t>CompTIA Pentest+ (Ethical Hacking) Course &amp; Practice Exam</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/linux-essentials-010/</t>
+  </si>
+  <si>
+    <t>LPI Linux Essentials (010-160) Complete Course and Exams</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/linux-essentials-practice-exams/</t>
+  </si>
+  <si>
+    <t>LPI Linux Essentials 010-160 (6 Practice Exams)</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/aws-certified-cloud-practitioner-practice-exams-c/</t>
+  </si>
+  <si>
+    <t>AWS Certified Cloud Practitioner 500 Practice Exam Questions</t>
   </si>
 </sst>
 </file>
@@ -846,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB6258B-92E2-456A-930B-3F7624ECCE6F}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -875,4 +900,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FC41BB-C39B-499C-AC2F-F0D039802BE5}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="119.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Django paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6525A8D8-F890-4D93-957E-ABC0C97559C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4C29F6-F66F-40E1-88B8-A2FBFC409F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="JavaScript" sheetId="6" r:id="rId6"/>
     <sheet name="API Dev and Testing" sheetId="7" r:id="rId7"/>
     <sheet name="Certification" sheetId="8" r:id="rId8"/>
+    <sheet name="Django" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -212,6 +213,36 @@
   </si>
   <si>
     <t>AWS Certified Cloud Practitioner 500 Practice Exam Questions</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/django-with-react-an-ecommerce-website/</t>
+  </si>
+  <si>
+    <t>Django with React | An Ecommerce Website</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/django-ecommerce-project-based-course-python-django-web-development/</t>
+  </si>
+  <si>
+    <t>Django Ecommerce | Build Advanced Django Web Application</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/python-django-the-practical-guide/</t>
+  </si>
+  <si>
+    <t>Python Django - The Practical Guide</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/develop-a-covid-19-live-web-app-with-python-django/</t>
+  </si>
+  <si>
+    <t>Develop A Covid-19 Live Web App With Python Django</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/python-django-tkinter-complete-bundle-advance/</t>
+  </si>
+  <si>
+    <t>Django &amp; Python: complete BUNDLE + Django real project 2020</t>
   </si>
 </sst>
 </file>
@@ -906,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FC41BB-C39B-499C-AC2F-F0D039802BE5}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -952,4 +983,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEFAF0C-E906-4FD3-8F47-37A381626B45}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="83.5703125" customWidth="1"/>
+    <col min="3" max="3" width="118.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AWS paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4C29F6-F66F-40E1-88B8-A2FBFC409F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C6BDE1-91E0-4656-9B8A-7B35D6D6BD03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="API Dev and Testing" sheetId="7" r:id="rId7"/>
     <sheet name="Certification" sheetId="8" r:id="rId8"/>
     <sheet name="Django" sheetId="9" r:id="rId9"/>
+    <sheet name="AWS" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -243,6 +244,36 @@
   </si>
   <si>
     <t>Django &amp; Python: complete BUNDLE + Django real project 2020</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/networking-in-aws/</t>
+  </si>
+  <si>
+    <t>AWS VPC and Networking in depth: Learn practically in 8 hrs</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/aws-with-python-and-boto3-managing-ec2-and-vpc/</t>
+  </si>
+  <si>
+    <t>Managing EC2 and VPC: AWS with Python and Boto3 Series</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/aws-automation-with-boto3-of-python-and-lambda-functions/</t>
+  </si>
+  <si>
+    <t>AWS Automation with boto3 of Python and Lambda Functions</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/aws-ec2-masterclass/</t>
+  </si>
+  <si>
+    <t>Amazon EC2 Master Class (with Auto Scaling &amp; Load Balancer)</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/hosting-websites-with-amazon-lightsail/</t>
+  </si>
+  <si>
+    <t>Hosting Websites with Amazon Lightsail | AWS for 2020</t>
   </si>
 </sst>
 </file>
@@ -643,6 +674,65 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8A0D4D-4ABE-4D87-BF01-51E2AB0D46C1}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6810214A-8824-42FE-A3A6-41C4FD4021BF}">
   <dimension ref="B2:C8"/>
@@ -989,7 +1079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEFAF0C-E906-4FD3-8F47-37A381626B45}">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Kotlin paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C6BDE1-91E0-4656-9B8A-7B35D6D6BD03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09865310-FF81-4840-9653-9957AD22CC30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Android Application" sheetId="2" r:id="rId2"/>
-    <sheet name="Python" sheetId="3" r:id="rId3"/>
-    <sheet name="Projects" sheetId="4" r:id="rId4"/>
-    <sheet name="Framework" sheetId="5" r:id="rId5"/>
-    <sheet name="JavaScript" sheetId="6" r:id="rId6"/>
-    <sheet name="API Dev and Testing" sheetId="7" r:id="rId7"/>
-    <sheet name="Certification" sheetId="8" r:id="rId8"/>
-    <sheet name="Django" sheetId="9" r:id="rId9"/>
-    <sheet name="AWS" sheetId="10" r:id="rId10"/>
+    <sheet name="Kotlin" sheetId="12" r:id="rId3"/>
+    <sheet name="Python" sheetId="3" r:id="rId4"/>
+    <sheet name="Projects" sheetId="4" r:id="rId5"/>
+    <sheet name="Framework" sheetId="5" r:id="rId6"/>
+    <sheet name="JavaScript" sheetId="6" r:id="rId7"/>
+    <sheet name="API Dev and Testing" sheetId="7" r:id="rId8"/>
+    <sheet name="Certification" sheetId="8" r:id="rId9"/>
+    <sheet name="Django" sheetId="9" r:id="rId10"/>
+    <sheet name="AWS" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -274,13 +275,25 @@
   </si>
   <si>
     <t>Hosting Websites with Amazon Lightsail | AWS for 2020</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/start-a-web-hosting-business/</t>
+  </si>
+  <si>
+    <t>How to Start and Run a Web Hosting Business from Home</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/the-complete-kotlin-developer-course-java/</t>
+  </si>
+  <si>
+    <t>The Complete Kotlin Developer Course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,13 +301,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,13 +331,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -625,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B039CD-88E5-4E86-BFC7-B084BD245489}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,16 +697,83 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEFAF0C-E906-4FD3-8F47-37A381626B45}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="83.5703125" customWidth="1"/>
+    <col min="3" max="3" width="118.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8A0D4D-4ABE-4D87-BF01-51E2AB0D46C1}">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -785,6 +880,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB64899B-2491-4CE5-9BED-F9FAFDF0E98C}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2773076E-175D-422E-B3B7-B91BC5516429}">
   <dimension ref="B2:C20"/>
   <sheetViews>
@@ -883,7 +1005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D41AAE-5841-4A02-8EA4-8A7C0835E48E}">
   <dimension ref="B2:C6"/>
   <sheetViews>
@@ -926,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD870DED-0179-42AB-8FFF-BE124EB6C140}">
   <dimension ref="B2:C4"/>
   <sheetViews>
@@ -961,7 +1083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C409B36-44BD-4ED2-A6DC-F7FC64FCD548}">
   <dimension ref="B2:C2"/>
   <sheetViews>
@@ -988,7 +1110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB6258B-92E2-456A-930B-3F7624ECCE6F}">
   <dimension ref="B2:C4"/>
   <sheetViews>
@@ -1023,7 +1145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FC41BB-C39B-499C-AC2F-F0D039802BE5}">
   <dimension ref="B2:C8"/>
   <sheetViews>
@@ -1073,63 +1195,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEFAF0C-E906-4FD3-8F47-37A381626B45}">
-  <dimension ref="B2:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="83.5703125" customWidth="1"/>
-    <col min="3" max="3" width="118.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
some more paid courses added.
</commit_message>
<xml_diff>
--- a/Udemy Courses.xlsx
+++ b/Udemy Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09865310-FF81-4840-9653-9957AD22CC30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE2626-9348-440D-8BFE-5480A9B09293}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89834C28-C284-4D05-9539-03B995E739D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>https://www.udemy.com/course/the-complete-introduction-to-c-programming/</t>
   </si>
@@ -287,6 +287,39 @@
   </si>
   <si>
     <t>The Complete Kotlin Developer Course</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/digital-electronics-logic-design/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/mongodb-the-complete-developers-guide/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/burp-suite-mastery-bug-hunters-perspective/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/practical-ethical-hacking/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/linux-mastery/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/build-10-c-beginner-projects-from-scratch/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/linux-privilege-escalation-for-beginners/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/learn-python-and-ethical-hacking-from-scratch/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/the-complete-nmap-ethical-hacking-course-network-security/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/advanced-css-and-sass/</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/responsive-web-design-tutorial-course-html5-css3-bootstrap/</t>
   </si>
 </sst>
 </file>
@@ -653,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B039CD-88E5-4E86-BFC7-B084BD245489}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="B2:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +736,61 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB64899B-2491-4CE5-9BED-F9FAFDF0E98C}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>